<commit_message>
Updated countries lat-long data and README
</commit_message>
<xml_diff>
--- a/Top_15_CO2_emissions_2009_Countries.xlsx
+++ b/Top_15_CO2_emissions_2009_Countries.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
   <si>
     <t>Rank</t>
   </si>
@@ -70,18 +70,30 @@
   </si>
   <si>
     <t>Australia</t>
+  </si>
+  <si>
+    <t>Latitude</t>
+  </si>
+  <si>
+    <t>Longitude</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF222222"/>
+      <name val="Calibri"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -105,8 +117,18 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -438,7 +460,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B16"/>
+  <dimension ref="A1:D16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A17" sqref="A17"/>
@@ -447,134 +469,232 @@
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="2" max="2" width="14.83203125" customWidth="1"/>
+    <col min="3" max="3" width="22" style="4" customWidth="1"/>
+    <col min="4" max="4" width="18.83203125" style="4" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
-      <c r="A1" t="s">
+    <row r="1" spans="1:4" s="1" customFormat="1">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:2">
-      <c r="A2">
+      <c r="C1" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" s="1" customFormat="1">
+      <c r="A2" s="1">
         <v>1</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="3" spans="1:2">
-      <c r="A3">
+      <c r="C2" s="3">
+        <v>35.861660000000001</v>
+      </c>
+      <c r="D2" s="3">
+        <v>104.195397</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" s="1" customFormat="1">
+      <c r="A3" s="1">
         <v>2</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="4" spans="1:2">
-      <c r="A4">
+      <c r="C3" s="2">
+        <v>37.090240000000001</v>
+      </c>
+      <c r="D3" s="2">
+        <v>-95.712890999999999</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" s="1" customFormat="1">
+      <c r="A4" s="1">
         <v>3</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="5" spans="1:2">
-      <c r="A5">
+      <c r="C4" s="3">
+        <v>20.593684</v>
+      </c>
+      <c r="D4" s="3">
+        <v>78.962879999999998</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" s="1" customFormat="1">
+      <c r="A5" s="1">
         <v>4</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" s="1" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="6" spans="1:2">
-      <c r="A6">
+      <c r="C5" s="3">
+        <v>61.524009999999997</v>
+      </c>
+      <c r="D5" s="3">
+        <v>105.31875599999999</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" s="1" customFormat="1">
+      <c r="A6" s="1">
         <v>5</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" s="1" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="7" spans="1:2">
-      <c r="A7">
+      <c r="C6" s="3">
+        <v>36.204824000000002</v>
+      </c>
+      <c r="D6" s="3">
+        <v>138.25292400000001</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" s="1" customFormat="1">
+      <c r="A7" s="1">
         <v>6</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B7" s="1" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="8" spans="1:2">
-      <c r="A8">
+      <c r="C7" s="3">
+        <v>51.165691000000002</v>
+      </c>
+      <c r="D7" s="3">
+        <v>10.451525999999999</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" s="1" customFormat="1">
+      <c r="A8" s="1">
         <v>7</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B8" s="1" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="9" spans="1:2">
-      <c r="A9">
+      <c r="C8" s="3">
+        <v>56.130366000000002</v>
+      </c>
+      <c r="D8" s="3">
+        <v>-106.346771</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" s="1" customFormat="1">
+      <c r="A9" s="1">
         <v>8</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B9" s="1" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="10" spans="1:2">
-      <c r="A10">
+      <c r="C9" s="3">
+        <v>35.907756999999997</v>
+      </c>
+      <c r="D9" s="3">
+        <v>127.76692199999999</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" s="1" customFormat="1">
+      <c r="A10" s="1">
         <v>9</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B10" s="1" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="11" spans="1:2">
-      <c r="A11">
+      <c r="C10" s="3">
+        <v>32.427908000000002</v>
+      </c>
+      <c r="D10" s="3">
+        <v>53.688046</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" s="1" customFormat="1">
+      <c r="A11" s="1">
         <v>10</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B11" s="1" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="12" spans="1:2">
-      <c r="A12">
+      <c r="C11" s="3">
+        <v>55.378050999999999</v>
+      </c>
+      <c r="D11" s="3">
+        <v>-3.4359730000000002</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" s="1" customFormat="1">
+      <c r="A12" s="1">
         <v>11</v>
       </c>
-      <c r="B12" t="s">
+      <c r="B12" s="1" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="13" spans="1:2">
-      <c r="A13">
+      <c r="C12" s="3">
+        <v>23.885942</v>
+      </c>
+      <c r="D12" s="3">
+        <v>45.079161999999997</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" s="1" customFormat="1">
+      <c r="A13" s="1">
         <v>12</v>
       </c>
-      <c r="B13" t="s">
+      <c r="B13" s="1" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="14" spans="1:2">
-      <c r="A14">
+      <c r="C13" s="3">
+        <v>-30.559481999999999</v>
+      </c>
+      <c r="D13" s="3">
+        <v>22.937505999999999</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" s="1" customFormat="1">
+      <c r="A14" s="1">
         <v>13</v>
       </c>
-      <c r="B14" t="s">
+      <c r="B14" s="1" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="15" spans="1:2">
-      <c r="A15">
+      <c r="C14" s="3">
+        <v>23.634501</v>
+      </c>
+      <c r="D14" s="3">
+        <v>-102.552784</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" s="1" customFormat="1">
+      <c r="A15" s="1">
         <v>14</v>
       </c>
-      <c r="B15" t="s">
+      <c r="B15" s="1" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="16" spans="1:2">
-      <c r="A16">
+      <c r="C15" s="3">
+        <v>-14.235004</v>
+      </c>
+      <c r="D15" s="3">
+        <v>-51.925280000000001</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" s="1" customFormat="1">
+      <c r="A16" s="1">
         <v>15</v>
       </c>
-      <c r="B16" t="s">
+      <c r="B16" s="1" t="s">
         <v>16</v>
+      </c>
+      <c r="C16" s="3">
+        <v>-25.274398000000001</v>
+      </c>
+      <c r="D16" s="3">
+        <v>133.775136</v>
       </c>
     </row>
   </sheetData>

</xml_diff>